<commit_message>
DS files and some improvement in xlsx tables
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb102/raw/Table7.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb102/raw/Table7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb102/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFE7C9C-2E04-5543-90ED-A0CBD3705BBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1E4B57-55D5-E744-A64E-81B617E925AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Region of residence</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Total check</t>
+  </si>
+  <si>
+    <t>Eureka</t>
   </si>
 </sst>
 </file>
@@ -80,7 +83,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -155,13 +158,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -482,16 +485,16 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="57"/>
     <col min="2" max="3" width="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,8 +505,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="B2" s="9">
         <v>836</v>
       </c>
@@ -577,7 +582,7 @@
         <v>3015</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -621,7 +626,7 @@
         <v>11647</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>

</xml_diff>